<commit_message>
real cash back 中的一个小bug
</commit_message>
<xml_diff>
--- a/iShangkeProject/Design/transform.xlsx
+++ b/iShangkeProject/Design/transform.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22905"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="38400" windowHeight="21600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="booking status " sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="150">
   <si>
     <t>状态名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -495,55 +495,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>支付成功</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>specialEnrolled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提交特卖支付</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>specialConfirm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待支付</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>specialCancelled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单取消</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>specialPayed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>specialConfirmed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单确认</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>specialPendingPayment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>specialEnroll</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>specialPendingPayment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>支付成功</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>specialEnrolled</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>订单完成</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提交特卖支付</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>specialConfirm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>待支付</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>specialCancelled</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>订单取消</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>specialPayed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>specialConfirmed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>订单确认</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -600,8 +604,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -617,9 +641,29 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="23">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -921,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1225,10 +1269,10 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="C28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1236,10 +1280,10 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1247,10 +1291,10 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1258,10 +1302,10 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C31" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1269,10 +1313,10 @@
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:1">
@@ -1284,6 +1328,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1296,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1639,7 +1684,7 @@
         <v>132</v>
       </c>
       <c r="C28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D28" t="s">
         <v>133</v>
@@ -1650,7 +1695,7 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C29" t="s">
         <v>135</v>
@@ -1664,10 +1709,10 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="C30" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D30" t="s">
         <v>134</v>

</xml_diff>